<commit_message>
fix agregar tarea, ya se limpia el formulario
</commit_message>
<xml_diff>
--- a/InformeTareas.xlsx
+++ b/InformeTareas.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>CATEGORÍA</t>
   </si>
@@ -27,39 +27,6 @@
   </si>
   <si>
     <t>FECHA</t>
-  </si>
-  <si>
-    <t>ejemplo de cate1</t>
-  </si>
-  <si>
-    <t>ejemplo de subcate1</t>
-  </si>
-  <si>
-    <t>recontramamabuebo bazo</t>
-  </si>
-  <si>
-    <t>2021-05-31 23:07:30</t>
-  </si>
-  <si>
-    <t>catejemplo 1</t>
-  </si>
-  <si>
-    <t>a ver que pasa</t>
-  </si>
-  <si>
-    <t>2021-06-23 20:33:32</t>
-  </si>
-  <si>
-    <t>describidita</t>
-  </si>
-  <si>
-    <t>2021-06-23 20:34:27</t>
-  </si>
-  <si>
-    <t>adad</t>
-  </si>
-  <si>
-    <t>2021-06-30 16:19:17</t>
   </si>
   <si>
     <t>Procesos internauticos</t>
@@ -84,28 +51,37 @@
     <t>2021-05-28 12:21:48</t>
   </si>
   <si>
+    <t>Pansensuales</t>
+  </si>
+  <si>
+    <t>Amo el pan</t>
+  </si>
+  <si>
+    <t>Esta descripción está super detallada ya que presenta sinopsis sinapticas en las mamalasticas</t>
+  </si>
+  <si>
+    <t>2021-05-26 12:31:52</t>
+  </si>
+  <si>
+    <t>Otra tarea dista mondá</t>
+  </si>
+  <si>
+    <t>2021-05-28 12:40:21</t>
+  </si>
+  <si>
     <t>Esta será la sexta tarea</t>
   </si>
   <si>
     <t>2021-05-26 17:34:19</t>
   </si>
   <si>
-    <t>Pansensuales</t>
-  </si>
-  <si>
-    <t>Amo el pan</t>
-  </si>
-  <si>
-    <t>Esta descripción está super detallada ya que presenta sinopsis sinapticas en las mamalasticas</t>
-  </si>
-  <si>
-    <t>2021-05-26 12:31:52</t>
-  </si>
-  <si>
-    <t>Otra tarea dista mondá</t>
-  </si>
-  <si>
-    <t>2021-05-28 12:40:21</t>
+    <t>Amo la mogolla</t>
+  </si>
+  <si>
+    <t>Tarea super genérica</t>
+  </si>
+  <si>
+    <t>2021-05-28 09:27:10</t>
   </si>
   <si>
     <t>BASADO recontramamabuebo</t>
@@ -114,25 +90,17 @@
     <t>2021-05-31 23:08:01</t>
   </si>
   <si>
-    <t>Amo la mogolla</t>
-  </si>
-  <si>
-    <t>Tarea super genérica</t>
-  </si>
-  <si>
-    <t>2021-05-28 09:27:10</t>
-  </si>
-  <si>
     <t>Phva pic</t>
   </si>
   <si>
     <t>Contratación</t>
   </si>
   <si>
-    <t>se realizó el documento</t>
-  </si>
-  <si>
-    <t>2021-06-02 21:05:10</t>
+    <t>se realizó el documento. 
+Mama guevo</t>
+  </si>
+  <si>
+    <t>2021-06-02 18:15:02</t>
   </si>
   <si>
     <t>Seguimiento</t>
@@ -142,6 +110,27 @@
   </si>
   <si>
     <t>2021-06-23 20:30:52</t>
+  </si>
+  <si>
+    <t>catejemplo 1</t>
+  </si>
+  <si>
+    <t>a ver que pasa</t>
+  </si>
+  <si>
+    <t>2021-06-23 20:33:32</t>
+  </si>
+  <si>
+    <t>1. phva pic</t>
+  </si>
+  <si>
+    <t>1. ejecución interno o alianzas</t>
+  </si>
+  <si>
+    <t>Prueba de mamarre</t>
+  </si>
+  <si>
+    <t>2021-08-08 18:37:57</t>
   </si>
 </sst>
 </file>
@@ -498,7 +487,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1:D1"/>
@@ -536,10 +525,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -550,38 +539,38 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -592,7 +581,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
@@ -606,10 +595,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
@@ -637,69 +626,41 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" t="s">
         <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>